<commit_message>
implemented proper handling of invalid submits (empty outputs)
</commit_message>
<xml_diff>
--- a/tmp/log_ASTIM.xlsx
+++ b/tmp/log_ASTIM.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Google Drive\PhD\NICE model\PyNICE\templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8295"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -27,6 +22,9 @@
     <t>Time</t>
   </si>
   <si>
+    <t>Neuron Type</t>
+  </si>
+  <si>
     <t>Radius (nm)</t>
   </si>
   <si>
@@ -66,33 +64,46 @@
     <t>Spike rate (sp/ms)</t>
   </si>
   <si>
-    <t>Neuron Type</t>
+    <t>2018.03.05</t>
+  </si>
+  <si>
+    <t>14:07:19</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>effective</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -108,25 +119,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -392,36 +394,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <selection activeCell="C1" pane="bottomLeft" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="9.5703125"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" width="7.7109375"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" width="12.42578125"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" width="11.5703125"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" width="14.42578125"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" width="11.5703125"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" width="11.85546875"/>
+    <col bestFit="1" customWidth="1" max="8" min="8" width="10.28515625"/>
+    <col bestFit="1" customWidth="1" max="9" min="9" width="9.28515625"/>
+    <col bestFit="1" customWidth="1" max="10" min="10" width="10.7109375"/>
+    <col bestFit="1" customWidth="1" max="11" min="11" width="9.5703125"/>
+    <col bestFit="1" customWidth="1" max="12" min="12" width="9.7109375"/>
+    <col bestFit="1" customWidth="1" max="13" min="13" width="14.140625"/>
+    <col bestFit="1" customWidth="1" max="14" min="14" width="8"/>
+    <col bestFit="1" customWidth="1" max="15" min="15" width="12.140625"/>
+    <col bestFit="1" customWidth="1" max="16" min="16" width="17.42578125"/>
+    <col bestFit="1" customWidth="1" max="19" min="19" width="18.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -429,50 +435,100 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="n">
+        <v>32</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G2" t="n">
+        <v>100</v>
+      </c>
+      <c r="H2" t="n">
+        <v>50</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="n">
+        <v>7000</v>
+      </c>
+      <c r="M2" t="n">
+        <v>5.99</v>
+      </c>
+      <c r="N2" t="n">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
+      <c r="O2" t="n">
+        <v>35.4</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.5423719619281825</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added red flashing of submit button in case of submit with invalid input parameters
</commit_message>
<xml_diff>
--- a/tmp/log_ASTIM.xlsx
+++ b/tmp/log_ASTIM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>effective</t>
+  </si>
+  <si>
+    <t>14:24:28</t>
   </si>
 </sst>
 </file>
@@ -399,7 +402,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
@@ -527,6 +530,56 @@
         <v>0.5423719619281825</v>
       </c>
     </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="n">
+        <v>32</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>100</v>
+      </c>
+      <c r="G3" t="n">
+        <v>100</v>
+      </c>
+      <c r="H3" t="n">
+        <v>50</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" t="n">
+        <v>7000</v>
+      </c>
+      <c r="M3" t="n">
+        <v>5.98</v>
+      </c>
+      <c r="N3" t="n">
+        <v>9</v>
+      </c>
+      <c r="O3" t="n">
+        <v>35.4</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.5423719619281825</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
adapted tool to new data in line with the paper.
</commit_message>
<xml_diff>
--- a/tmp/log_ASTIM.xlsx
+++ b/tmp/log_ASTIM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -80,6 +80,18 @@
   </si>
   <si>
     <t>14:24:28</t>
+  </si>
+  <si>
+    <t>2018.07.04</t>
+  </si>
+  <si>
+    <t>15:02:44</t>
+  </si>
+  <si>
+    <t>15:04:31</t>
+  </si>
+  <si>
+    <t>15:04:50</t>
   </si>
 </sst>
 </file>
@@ -402,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
@@ -580,6 +592,156 @@
         <v>0.5423719619281825</v>
       </c>
     </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="n">
+        <v>32</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>100</v>
+      </c>
+      <c r="G4" t="n">
+        <v>102</v>
+      </c>
+      <c r="H4" t="n">
+        <v>250</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.0095</v>
+      </c>
+      <c r="K4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" t="n">
+        <v>7000</v>
+      </c>
+      <c r="M4" t="n">
+        <v>3.19</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="n">
+        <v>32</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>100</v>
+      </c>
+      <c r="G5" t="n">
+        <v>99</v>
+      </c>
+      <c r="H5" t="n">
+        <v>250</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="K5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" t="n">
+        <v>7000</v>
+      </c>
+      <c r="M5" t="n">
+        <v>8.56</v>
+      </c>
+      <c r="N5" t="n">
+        <v>111</v>
+      </c>
+      <c r="O5" t="n">
+        <v>36.7</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.5385884953938632</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="n">
+        <v>32</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>4000</v>
+      </c>
+      <c r="G6" t="n">
+        <v>99</v>
+      </c>
+      <c r="H6" t="n">
+        <v>250</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="K6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" t="n">
+        <v>7000</v>
+      </c>
+      <c r="M6" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="N6" t="n">
+        <v>81</v>
+      </c>
+      <c r="O6" t="n">
+        <v>43.85</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.4066105357283207</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
corrected home page typo. added mention of Dash.
</commit_message>
<xml_diff>
--- a/tmp/log_ASTIM.xlsx
+++ b/tmp/log_ASTIM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -92,6 +92,12 @@
   </si>
   <si>
     <t>15:04:50</t>
+  </si>
+  <si>
+    <t>2018.07.05</t>
+  </si>
+  <si>
+    <t>12:22:01</t>
   </si>
 </sst>
 </file>
@@ -414,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
@@ -742,6 +748,56 @@
         <v>0.4066105357283207</v>
       </c>
     </row>
+    <row r="7" spans="1:16">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="n">
+        <v>32</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>100</v>
+      </c>
+      <c r="G7" t="n">
+        <v>100</v>
+      </c>
+      <c r="H7" t="n">
+        <v>250</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" t="n">
+        <v>7000</v>
+      </c>
+      <c r="M7" t="n">
+        <v>9.08</v>
+      </c>
+      <c r="N7" t="n">
+        <v>117</v>
+      </c>
+      <c r="O7" t="n">
+        <v>35.4</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.5413239918684565</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
changed name to WebSONIC, updated dependency on PySONIC.
</commit_message>
<xml_diff>
--- a/tmp/log_ASTIM.xlsx
+++ b/tmp/log_ASTIM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -98,6 +98,15 @@
   </si>
   <si>
     <t>12:22:01</t>
+  </si>
+  <si>
+    <t>2018.08.21</t>
+  </si>
+  <si>
+    <t>16:54:35</t>
+  </si>
+  <si>
+    <t>16:57:13</t>
   </si>
 </sst>
 </file>
@@ -420,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
@@ -798,6 +807,106 @@
         <v>0.5413239918684565</v>
       </c>
     </row>
+    <row r="8" spans="1:16">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="n">
+        <v>32</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>100</v>
+      </c>
+      <c r="G8" t="n">
+        <v>100</v>
+      </c>
+      <c r="H8" t="n">
+        <v>250</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="K8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" t="n">
+        <v>7000</v>
+      </c>
+      <c r="M8" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="N8" t="n">
+        <v>66</v>
+      </c>
+      <c r="O8" t="n">
+        <v>37.04999999999999</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.4798719937468688</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="n">
+        <v>32</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>100</v>
+      </c>
+      <c r="G9" t="n">
+        <v>100</v>
+      </c>
+      <c r="H9" t="n">
+        <v>250</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="K9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" t="n">
+        <v>7000</v>
+      </c>
+      <c r="M9" t="n">
+        <v>9.08</v>
+      </c>
+      <c r="N9" t="n">
+        <v>118</v>
+      </c>
+      <c r="O9" t="n">
+        <v>36.4</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.5507834180841099</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
Major update: re-implemented the app in object-oriented way, and turned it into a package.
</commit_message>
<xml_diff>
--- a/tmp/log_ASTIM.xlsx
+++ b/tmp/log_ASTIM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -107,6 +107,30 @@
   </si>
   <si>
     <t>16:57:13</t>
+  </si>
+  <si>
+    <t>2018.08.23</t>
+  </si>
+  <si>
+    <t>18:45:03</t>
+  </si>
+  <si>
+    <t>18:50:13</t>
+  </si>
+  <si>
+    <t>19:04:08</t>
+  </si>
+  <si>
+    <t>2018.08.24</t>
+  </si>
+  <si>
+    <t>16:37:39</t>
+  </si>
+  <si>
+    <t>16:39:50</t>
+  </si>
+  <si>
+    <t>16:42:28</t>
   </si>
 </sst>
 </file>
@@ -429,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
@@ -907,6 +931,306 @@
         <v>0.5507834180841099</v>
       </c>
     </row>
+    <row r="10" spans="1:16">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="n">
+        <v>32</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>2010</v>
+      </c>
+      <c r="G10" t="n">
+        <v>305</v>
+      </c>
+      <c r="H10" t="n">
+        <v>250</v>
+      </c>
+      <c r="I10" t="n">
+        <v>5.005</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.505</v>
+      </c>
+      <c r="K10" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" t="n">
+        <v>6004</v>
+      </c>
+      <c r="M10" t="n">
+        <v>16.06</v>
+      </c>
+      <c r="N10" t="n">
+        <v>181</v>
+      </c>
+      <c r="O10" t="n">
+        <v>40.95904095904093</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.8630950329170262</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="n">
+        <v>32</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>500</v>
+      </c>
+      <c r="G11" t="n">
+        <v>100</v>
+      </c>
+      <c r="H11" t="n">
+        <v>250</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.9500000000000001</v>
+      </c>
+      <c r="K11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" t="n">
+        <v>6000</v>
+      </c>
+      <c r="M11" t="n">
+        <v>9.17</v>
+      </c>
+      <c r="N11" t="n">
+        <v>78</v>
+      </c>
+      <c r="O11" t="n">
+        <v>37.1</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.4857362089357296</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="n">
+        <v>32</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>500</v>
+      </c>
+      <c r="G12" t="n">
+        <v>100</v>
+      </c>
+      <c r="H12" t="n">
+        <v>250</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="K12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L12" t="n">
+        <v>6000</v>
+      </c>
+      <c r="M12" t="n">
+        <v>8.039999999999999</v>
+      </c>
+      <c r="N12" t="n">
+        <v>60</v>
+      </c>
+      <c r="O12" t="n">
+        <v>39.09999999999999</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.4846200285278927</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="n">
+        <v>32</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>500</v>
+      </c>
+      <c r="G13" t="n">
+        <v>100</v>
+      </c>
+      <c r="H13" t="n">
+        <v>250</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="K13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" t="n">
+        <v>6000</v>
+      </c>
+      <c r="M13" t="n">
+        <v>9.720000000000001</v>
+      </c>
+      <c r="N13" t="n">
+        <v>85</v>
+      </c>
+      <c r="O13" t="n">
+        <v>36.8</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.4878273340644669</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="n">
+        <v>32</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>500</v>
+      </c>
+      <c r="G14" t="n">
+        <v>95</v>
+      </c>
+      <c r="H14" t="n">
+        <v>250</v>
+      </c>
+      <c r="I14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" t="n">
+        <v>6000</v>
+      </c>
+      <c r="M14" t="n">
+        <v>10.79</v>
+      </c>
+      <c r="N14" t="n">
+        <v>111</v>
+      </c>
+      <c r="O14" t="n">
+        <v>37.05</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.515805960224653</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="n">
+        <v>32</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>500</v>
+      </c>
+      <c r="G15" t="n">
+        <v>11</v>
+      </c>
+      <c r="H15" t="n">
+        <v>250</v>
+      </c>
+      <c r="I15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L15" t="n">
+        <v>6000</v>
+      </c>
+      <c r="M15" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="s">
+        <v>19</v>
+      </c>
+      <c r="P15" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
changed submit button style
</commit_message>
<xml_diff>
--- a/tmp/log_ASTIM.xlsx
+++ b/tmp/log_ASTIM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
   <si>
     <t>Date</t>
   </si>
@@ -131,6 +131,21 @@
   </si>
   <si>
     <t>16:42:28</t>
+  </si>
+  <si>
+    <t>19:57:16</t>
+  </si>
+  <si>
+    <t>20:05:09</t>
+  </si>
+  <si>
+    <t>20:08:04</t>
+  </si>
+  <si>
+    <t>20:08:24</t>
+  </si>
+  <si>
+    <t>20:15:23</t>
   </si>
 </sst>
 </file>
@@ -453,7 +468,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
@@ -1231,6 +1246,256 @@
         <v>19</v>
       </c>
     </row>
+    <row r="16" spans="1:16">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" t="n">
+        <v>32</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>500</v>
+      </c>
+      <c r="G16" t="n">
+        <v>100</v>
+      </c>
+      <c r="H16" t="n">
+        <v>250</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.9500000000000001</v>
+      </c>
+      <c r="K16" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" t="n">
+        <v>6000</v>
+      </c>
+      <c r="M16" t="n">
+        <v>9.800000000000001</v>
+      </c>
+      <c r="N16" t="n">
+        <v>78</v>
+      </c>
+      <c r="O16" t="n">
+        <v>37.1</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.4857362089357296</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="n">
+        <v>32</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>500</v>
+      </c>
+      <c r="G17" t="n">
+        <v>100</v>
+      </c>
+      <c r="H17" t="n">
+        <v>250</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="K17" t="s">
+        <v>20</v>
+      </c>
+      <c r="L17" t="n">
+        <v>6000</v>
+      </c>
+      <c r="M17" t="n">
+        <v>7.58</v>
+      </c>
+      <c r="N17" t="n">
+        <v>49</v>
+      </c>
+      <c r="O17" t="n">
+        <v>38.55</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.4479769510540157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" t="n">
+        <v>32</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>500</v>
+      </c>
+      <c r="G18" t="n">
+        <v>100</v>
+      </c>
+      <c r="H18" t="n">
+        <v>250</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.9500000000000001</v>
+      </c>
+      <c r="K18" t="s">
+        <v>20</v>
+      </c>
+      <c r="L18" t="n">
+        <v>6000</v>
+      </c>
+      <c r="M18" t="n">
+        <v>9.49</v>
+      </c>
+      <c r="N18" t="n">
+        <v>78</v>
+      </c>
+      <c r="O18" t="n">
+        <v>37.1</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.4857362089357296</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" t="n">
+        <v>32</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>500</v>
+      </c>
+      <c r="G19" t="n">
+        <v>100</v>
+      </c>
+      <c r="H19" t="n">
+        <v>250</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="K19" t="s">
+        <v>20</v>
+      </c>
+      <c r="L19" t="n">
+        <v>6000</v>
+      </c>
+      <c r="M19" t="n">
+        <v>7.48</v>
+      </c>
+      <c r="N19" t="n">
+        <v>47</v>
+      </c>
+      <c r="O19" t="n">
+        <v>38.15000000000001</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.4599823614175941</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" t="n">
+        <v>32</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>500</v>
+      </c>
+      <c r="G20" t="n">
+        <v>100</v>
+      </c>
+      <c r="H20" t="n">
+        <v>250</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="K20" t="s">
+        <v>20</v>
+      </c>
+      <c r="L20" t="n">
+        <v>6000</v>
+      </c>
+      <c r="M20" t="n">
+        <v>9.460000000000001</v>
+      </c>
+      <c r="N20" t="n">
+        <v>85</v>
+      </c>
+      <c r="O20" t="n">
+        <v>36.8</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0.4878273340644669</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
cleaned up SONICViewer initialization. added http authentification option as run.py command line argument. added favicon.
</commit_message>
<xml_diff>
--- a/tmp/log_ASTIM.xlsx
+++ b/tmp/log_ASTIM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -146,6 +146,27 @@
   </si>
   <si>
     <t>20:15:23</t>
+  </si>
+  <si>
+    <t>2018.08.27</t>
+  </si>
+  <si>
+    <t>16:23:13</t>
+  </si>
+  <si>
+    <t>sonic</t>
+  </si>
+  <si>
+    <t>16:25:54</t>
+  </si>
+  <si>
+    <t>17:21:14</t>
+  </si>
+  <si>
+    <t>17:24:37</t>
+  </si>
+  <si>
+    <t>17:31:04</t>
   </si>
 </sst>
 </file>
@@ -468,7 +489,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
@@ -1496,6 +1517,256 @@
         <v>0.4878273340644669</v>
       </c>
     </row>
+    <row r="21" spans="1:16">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" t="n">
+        <v>32</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>500</v>
+      </c>
+      <c r="G21" t="n">
+        <v>100</v>
+      </c>
+      <c r="H21" t="n">
+        <v>250</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.9400000000000001</v>
+      </c>
+      <c r="K21" t="s">
+        <v>46</v>
+      </c>
+      <c r="L21" t="n">
+        <v>6000</v>
+      </c>
+      <c r="M21" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="N21" t="n">
+        <v>61</v>
+      </c>
+      <c r="O21" t="n">
+        <v>37.45</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0.4808171216961022</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" t="n">
+        <v>32</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>500</v>
+      </c>
+      <c r="G22" t="n">
+        <v>100</v>
+      </c>
+      <c r="H22" t="n">
+        <v>250</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="K22" t="s">
+        <v>46</v>
+      </c>
+      <c r="L22" t="n">
+        <v>6000</v>
+      </c>
+      <c r="M22" t="n">
+        <v>9.32</v>
+      </c>
+      <c r="N22" t="n">
+        <v>85</v>
+      </c>
+      <c r="O22" t="n">
+        <v>36.8</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0.4878273340644669</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" t="n">
+        <v>32</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>500</v>
+      </c>
+      <c r="G23" t="n">
+        <v>100</v>
+      </c>
+      <c r="H23" t="n">
+        <v>250</v>
+      </c>
+      <c r="I23" t="s">
+        <v>19</v>
+      </c>
+      <c r="J23" t="n">
+        <v>1</v>
+      </c>
+      <c r="K23" t="s">
+        <v>46</v>
+      </c>
+      <c r="L23" t="n">
+        <v>6000</v>
+      </c>
+      <c r="M23" t="n">
+        <v>10.84</v>
+      </c>
+      <c r="N23" t="n">
+        <v>114</v>
+      </c>
+      <c r="O23" t="n">
+        <v>35.8</v>
+      </c>
+      <c r="P23" t="n">
+        <v>0.5267293749593411</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" t="n">
+        <v>32</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>500</v>
+      </c>
+      <c r="G24" t="n">
+        <v>100</v>
+      </c>
+      <c r="H24" t="n">
+        <v>250</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="K24" t="s">
+        <v>46</v>
+      </c>
+      <c r="L24" t="n">
+        <v>6000</v>
+      </c>
+      <c r="M24" t="n">
+        <v>7.22</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0</v>
+      </c>
+      <c r="O24" t="s">
+        <v>19</v>
+      </c>
+      <c r="P24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" t="n">
+        <v>32</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>500</v>
+      </c>
+      <c r="G25" t="n">
+        <v>100</v>
+      </c>
+      <c r="H25" t="n">
+        <v>250</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.9500000000000001</v>
+      </c>
+      <c r="K25" t="s">
+        <v>46</v>
+      </c>
+      <c r="L25" t="n">
+        <v>6000</v>
+      </c>
+      <c r="M25" t="n">
+        <v>8.84</v>
+      </c>
+      <c r="N25" t="n">
+        <v>78</v>
+      </c>
+      <c r="O25" t="n">
+        <v>37.1</v>
+      </c>
+      <c r="P25" t="n">
+        <v>0.4857362089357296</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
Implemented data update from on-the-fly NEURON simulations (removed SSH connection with remote data server).
</commit_message>
<xml_diff>
--- a/tmp/log_ASTIM.xlsx
+++ b/tmp/log_ASTIM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="99">
   <si>
     <t>Date</t>
   </si>
@@ -167,6 +167,150 @@
   </si>
   <si>
     <t>17:31:04</t>
+  </si>
+  <si>
+    <t>2018.08.30</t>
+  </si>
+  <si>
+    <t>15:36:32</t>
+  </si>
+  <si>
+    <t>NEURON</t>
+  </si>
+  <si>
+    <t>15:38:11</t>
+  </si>
+  <si>
+    <t>15:39:09</t>
+  </si>
+  <si>
+    <t>15:39:15</t>
+  </si>
+  <si>
+    <t>15:39:23</t>
+  </si>
+  <si>
+    <t>15:39:25</t>
+  </si>
+  <si>
+    <t>15:39:29</t>
+  </si>
+  <si>
+    <t>15:39:31</t>
+  </si>
+  <si>
+    <t>15:39:33</t>
+  </si>
+  <si>
+    <t>15:39:34</t>
+  </si>
+  <si>
+    <t>15:39:36</t>
+  </si>
+  <si>
+    <t>15:41:34</t>
+  </si>
+  <si>
+    <t>15:41:41</t>
+  </si>
+  <si>
+    <t>15:43:42</t>
+  </si>
+  <si>
+    <t>15:43:47</t>
+  </si>
+  <si>
+    <t>16:17:01</t>
+  </si>
+  <si>
+    <t>16:17:12</t>
+  </si>
+  <si>
+    <t>16:17:20</t>
+  </si>
+  <si>
+    <t>16:17:28</t>
+  </si>
+  <si>
+    <t>16:20:01</t>
+  </si>
+  <si>
+    <t>16:20:07</t>
+  </si>
+  <si>
+    <t>16:20:12</t>
+  </si>
+  <si>
+    <t>16:20:14</t>
+  </si>
+  <si>
+    <t>16:20:16</t>
+  </si>
+  <si>
+    <t>16:20:21</t>
+  </si>
+  <si>
+    <t>16:29:24</t>
+  </si>
+  <si>
+    <t>16:29:48</t>
+  </si>
+  <si>
+    <t>16:29:58</t>
+  </si>
+  <si>
+    <t>16:30:14</t>
+  </si>
+  <si>
+    <t>16:30:18</t>
+  </si>
+  <si>
+    <t>16:30:20</t>
+  </si>
+  <si>
+    <t>16:30:23</t>
+  </si>
+  <si>
+    <t>16:30:26</t>
+  </si>
+  <si>
+    <t>16:36:59</t>
+  </si>
+  <si>
+    <t>16:37:35</t>
+  </si>
+  <si>
+    <t>16:37:45</t>
+  </si>
+  <si>
+    <t>16:39:08</t>
+  </si>
+  <si>
+    <t>16:39:10</t>
+  </si>
+  <si>
+    <t>16:39:41</t>
+  </si>
+  <si>
+    <t>16:42:35</t>
+  </si>
+  <si>
+    <t>16:59:30</t>
+  </si>
+  <si>
+    <t>17:00:25</t>
+  </si>
+  <si>
+    <t>17:00:31</t>
+  </si>
+  <si>
+    <t>17:00:33</t>
+  </si>
+  <si>
+    <t>17:00:41</t>
+  </si>
+  <si>
+    <t>17:00:47</t>
   </si>
 </sst>
 </file>
@@ -489,7 +633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:P71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
@@ -1767,6 +1911,2306 @@
         <v>0.4857362089357296</v>
       </c>
     </row>
+    <row r="26" spans="1:16">
+      <c r="A26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" t="n">
+        <v>32</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>500</v>
+      </c>
+      <c r="G26" t="n">
+        <v>100</v>
+      </c>
+      <c r="H26" t="n">
+        <v>250</v>
+      </c>
+      <c r="I26" t="s">
+        <v>19</v>
+      </c>
+      <c r="J26" t="n">
+        <v>1</v>
+      </c>
+      <c r="K26" t="s">
+        <v>53</v>
+      </c>
+      <c r="L26" t="n">
+        <v>10335</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.2131</v>
+      </c>
+      <c r="N26" t="n">
+        <v>4</v>
+      </c>
+      <c r="O26" t="n">
+        <v>35.78592371085093</v>
+      </c>
+      <c r="P26" t="n">
+        <v>0.0144471012717442</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" t="n">
+        <v>32</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>500</v>
+      </c>
+      <c r="G27" t="n">
+        <v>100</v>
+      </c>
+      <c r="H27" t="n">
+        <v>250</v>
+      </c>
+      <c r="I27" t="s">
+        <v>19</v>
+      </c>
+      <c r="J27" t="n">
+        <v>1</v>
+      </c>
+      <c r="K27" t="s">
+        <v>53</v>
+      </c>
+      <c r="L27" t="n">
+        <v>10335</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0.195</v>
+      </c>
+      <c r="N27" t="n">
+        <v>4</v>
+      </c>
+      <c r="O27" t="n">
+        <v>35.78592371085093</v>
+      </c>
+      <c r="P27" t="n">
+        <v>0.0144471012717442</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" t="n">
+        <v>32</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>500</v>
+      </c>
+      <c r="G28" t="n">
+        <v>100</v>
+      </c>
+      <c r="H28" t="n">
+        <v>250</v>
+      </c>
+      <c r="I28" t="s">
+        <v>19</v>
+      </c>
+      <c r="J28" t="n">
+        <v>1</v>
+      </c>
+      <c r="K28" t="s">
+        <v>53</v>
+      </c>
+      <c r="L28" t="n">
+        <v>10335</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0.191</v>
+      </c>
+      <c r="N28" t="n">
+        <v>4</v>
+      </c>
+      <c r="O28" t="n">
+        <v>35.78592371085093</v>
+      </c>
+      <c r="P28" t="n">
+        <v>0.0144471012717442</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" t="n">
+        <v>32</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>500</v>
+      </c>
+      <c r="G29" t="n">
+        <v>300</v>
+      </c>
+      <c r="H29" t="n">
+        <v>250</v>
+      </c>
+      <c r="I29" t="s">
+        <v>19</v>
+      </c>
+      <c r="J29" t="n">
+        <v>1</v>
+      </c>
+      <c r="K29" t="s">
+        <v>53</v>
+      </c>
+      <c r="L29" t="n">
+        <v>12816</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0.1725</v>
+      </c>
+      <c r="N29" t="n">
+        <v>1</v>
+      </c>
+      <c r="O29" t="n">
+        <v>250.3291628551787</v>
+      </c>
+      <c r="P29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" t="n">
+        <v>32</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>500</v>
+      </c>
+      <c r="G30" t="n">
+        <v>300</v>
+      </c>
+      <c r="H30" t="n">
+        <v>250</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="K30" t="s">
+        <v>53</v>
+      </c>
+      <c r="L30" t="n">
+        <v>980</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0.0321</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" t="s">
+        <v>19</v>
+      </c>
+      <c r="P30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" t="n">
+        <v>32</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>500</v>
+      </c>
+      <c r="G31" t="n">
+        <v>300</v>
+      </c>
+      <c r="H31" t="n">
+        <v>250</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K31" t="s">
+        <v>53</v>
+      </c>
+      <c r="L31" t="n">
+        <v>2494</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0.0546</v>
+      </c>
+      <c r="N31" t="n">
+        <v>1</v>
+      </c>
+      <c r="O31" t="n">
+        <v>35.80563434032669</v>
+      </c>
+      <c r="P31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" t="n">
+        <v>32</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>500</v>
+      </c>
+      <c r="G32" t="n">
+        <v>300</v>
+      </c>
+      <c r="H32" t="n">
+        <v>250</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="K32" t="s">
+        <v>53</v>
+      </c>
+      <c r="L32" t="n">
+        <v>4046</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0.06469999999999999</v>
+      </c>
+      <c r="N32" t="n">
+        <v>1</v>
+      </c>
+      <c r="O32" t="n">
+        <v>208.0402794253428</v>
+      </c>
+      <c r="P32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" t="n">
+        <v>32</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>500</v>
+      </c>
+      <c r="G33" t="n">
+        <v>300</v>
+      </c>
+      <c r="H33" t="n">
+        <v>250</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K33" t="s">
+        <v>53</v>
+      </c>
+      <c r="L33" t="n">
+        <v>931</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0.0276</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0</v>
+      </c>
+      <c r="O33" t="s">
+        <v>19</v>
+      </c>
+      <c r="P33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" t="n">
+        <v>32</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>500</v>
+      </c>
+      <c r="G34" t="n">
+        <v>300</v>
+      </c>
+      <c r="H34" t="n">
+        <v>250</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="K34" t="s">
+        <v>53</v>
+      </c>
+      <c r="L34" t="n">
+        <v>980</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0.0281</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0</v>
+      </c>
+      <c r="O34" t="s">
+        <v>19</v>
+      </c>
+      <c r="P34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" t="n">
+        <v>32</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>500</v>
+      </c>
+      <c r="G35" t="n">
+        <v>300</v>
+      </c>
+      <c r="H35" t="n">
+        <v>250</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="K35" t="s">
+        <v>53</v>
+      </c>
+      <c r="L35" t="n">
+        <v>1742</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0.0406</v>
+      </c>
+      <c r="N35" t="n">
+        <v>1</v>
+      </c>
+      <c r="O35" t="n">
+        <v>89.15633196313479</v>
+      </c>
+      <c r="P35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
+      <c r="A36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" t="s">
+        <v>63</v>
+      </c>
+      <c r="C36" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" t="n">
+        <v>32</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>500</v>
+      </c>
+      <c r="G36" t="n">
+        <v>300</v>
+      </c>
+      <c r="H36" t="n">
+        <v>250</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="K36" t="s">
+        <v>53</v>
+      </c>
+      <c r="L36" t="n">
+        <v>4046</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0.0672</v>
+      </c>
+      <c r="N36" t="n">
+        <v>1</v>
+      </c>
+      <c r="O36" t="n">
+        <v>208.0402794253428</v>
+      </c>
+      <c r="P36" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
+      <c r="A37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" t="n">
+        <v>32</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>500</v>
+      </c>
+      <c r="G37" t="n">
+        <v>100</v>
+      </c>
+      <c r="H37" t="n">
+        <v>250</v>
+      </c>
+      <c r="I37" t="s">
+        <v>19</v>
+      </c>
+      <c r="J37" t="n">
+        <v>1</v>
+      </c>
+      <c r="K37" t="s">
+        <v>53</v>
+      </c>
+      <c r="L37" t="n">
+        <v>10335</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0.206</v>
+      </c>
+      <c r="N37" t="n">
+        <v>4</v>
+      </c>
+      <c r="O37" t="n">
+        <v>35.78592371085093</v>
+      </c>
+      <c r="P37" t="n">
+        <v>0.0144471012717442</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
+      <c r="A38" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" t="n">
+        <v>32</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" t="n">
+        <v>500</v>
+      </c>
+      <c r="G38" t="n">
+        <v>100</v>
+      </c>
+      <c r="H38" t="n">
+        <v>250</v>
+      </c>
+      <c r="I38" t="s">
+        <v>19</v>
+      </c>
+      <c r="J38" t="n">
+        <v>1</v>
+      </c>
+      <c r="K38" t="s">
+        <v>53</v>
+      </c>
+      <c r="L38" t="n">
+        <v>10335</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0.1511</v>
+      </c>
+      <c r="N38" t="n">
+        <v>4</v>
+      </c>
+      <c r="O38" t="n">
+        <v>35.78592371085093</v>
+      </c>
+      <c r="P38" t="n">
+        <v>0.0144471012717442</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
+      <c r="A39" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" t="n">
+        <v>32</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>500</v>
+      </c>
+      <c r="G39" t="n">
+        <v>100</v>
+      </c>
+      <c r="H39" t="n">
+        <v>250</v>
+      </c>
+      <c r="I39" t="s">
+        <v>19</v>
+      </c>
+      <c r="J39" t="n">
+        <v>1</v>
+      </c>
+      <c r="K39" t="s">
+        <v>53</v>
+      </c>
+      <c r="L39" t="n">
+        <v>10335</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0.189</v>
+      </c>
+      <c r="N39" t="n">
+        <v>4</v>
+      </c>
+      <c r="O39" t="n">
+        <v>35.78592371085093</v>
+      </c>
+      <c r="P39" t="n">
+        <v>0.0144471012717442</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
+      <c r="A40" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" t="n">
+        <v>32</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>500</v>
+      </c>
+      <c r="G40" t="n">
+        <v>100</v>
+      </c>
+      <c r="H40" t="n">
+        <v>250</v>
+      </c>
+      <c r="I40" t="s">
+        <v>19</v>
+      </c>
+      <c r="J40" t="n">
+        <v>1</v>
+      </c>
+      <c r="K40" t="s">
+        <v>53</v>
+      </c>
+      <c r="L40" t="n">
+        <v>10335</v>
+      </c>
+      <c r="M40" t="n">
+        <v>0.1519</v>
+      </c>
+      <c r="N40" t="n">
+        <v>4</v>
+      </c>
+      <c r="O40" t="n">
+        <v>35.78592371085093</v>
+      </c>
+      <c r="P40" t="n">
+        <v>0.0144471012717442</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
+      <c r="A41" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" t="n">
+        <v>32</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" t="n">
+        <v>500</v>
+      </c>
+      <c r="G41" t="n">
+        <v>100</v>
+      </c>
+      <c r="H41" t="n">
+        <v>250</v>
+      </c>
+      <c r="I41" t="s">
+        <v>19</v>
+      </c>
+      <c r="J41" t="n">
+        <v>1</v>
+      </c>
+      <c r="K41" t="s">
+        <v>53</v>
+      </c>
+      <c r="L41" t="n">
+        <v>10335</v>
+      </c>
+      <c r="M41" t="n">
+        <v>0.205</v>
+      </c>
+      <c r="N41" t="n">
+        <v>4</v>
+      </c>
+      <c r="O41" t="n">
+        <v>35.78592371085093</v>
+      </c>
+      <c r="P41" t="n">
+        <v>0.0144471012717442</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
+      <c r="A42" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" t="n">
+        <v>32</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" t="n">
+        <v>500</v>
+      </c>
+      <c r="G42" t="n">
+        <v>300</v>
+      </c>
+      <c r="H42" t="n">
+        <v>250</v>
+      </c>
+      <c r="I42" t="s">
+        <v>19</v>
+      </c>
+      <c r="J42" t="n">
+        <v>1</v>
+      </c>
+      <c r="K42" t="s">
+        <v>53</v>
+      </c>
+      <c r="L42" t="n">
+        <v>12816</v>
+      </c>
+      <c r="M42" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="N42" t="n">
+        <v>1</v>
+      </c>
+      <c r="O42" t="n">
+        <v>250.3291628551787</v>
+      </c>
+      <c r="P42" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
+      <c r="A43" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" t="n">
+        <v>32</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" t="n">
+        <v>500</v>
+      </c>
+      <c r="G43" t="n">
+        <v>300</v>
+      </c>
+      <c r="H43" t="n">
+        <v>250</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="K43" t="s">
+        <v>53</v>
+      </c>
+      <c r="L43" t="n">
+        <v>1742</v>
+      </c>
+      <c r="M43" t="n">
+        <v>0.0416</v>
+      </c>
+      <c r="N43" t="n">
+        <v>1</v>
+      </c>
+      <c r="O43" t="n">
+        <v>89.15633196313479</v>
+      </c>
+      <c r="P43" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
+      <c r="A44" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" t="n">
+        <v>32</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" t="n">
+        <v>500</v>
+      </c>
+      <c r="G44" t="n">
+        <v>300</v>
+      </c>
+      <c r="H44" t="n">
+        <v>250</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J44" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="K44" t="s">
+        <v>53</v>
+      </c>
+      <c r="L44" t="n">
+        <v>1742</v>
+      </c>
+      <c r="M44" t="n">
+        <v>0.0386</v>
+      </c>
+      <c r="N44" t="n">
+        <v>1</v>
+      </c>
+      <c r="O44" t="n">
+        <v>89.15633196313479</v>
+      </c>
+      <c r="P44" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
+      <c r="A45" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" t="s">
+        <v>72</v>
+      </c>
+      <c r="C45" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" t="n">
+        <v>32</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>500</v>
+      </c>
+      <c r="G45" t="n">
+        <v>100</v>
+      </c>
+      <c r="H45" t="n">
+        <v>250</v>
+      </c>
+      <c r="I45" t="s">
+        <v>19</v>
+      </c>
+      <c r="J45" t="n">
+        <v>1</v>
+      </c>
+      <c r="K45" t="s">
+        <v>53</v>
+      </c>
+      <c r="L45" t="n">
+        <v>10335</v>
+      </c>
+      <c r="M45" t="n">
+        <v>0.1831</v>
+      </c>
+      <c r="N45" t="n">
+        <v>4</v>
+      </c>
+      <c r="O45" t="n">
+        <v>35.78592371085093</v>
+      </c>
+      <c r="P45" t="n">
+        <v>0.0144471012717442</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
+      <c r="A46" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" t="s">
+        <v>73</v>
+      </c>
+      <c r="C46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" t="n">
+        <v>32</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" t="n">
+        <v>500</v>
+      </c>
+      <c r="G46" t="n">
+        <v>300</v>
+      </c>
+      <c r="H46" t="n">
+        <v>250</v>
+      </c>
+      <c r="I46" t="s">
+        <v>19</v>
+      </c>
+      <c r="J46" t="n">
+        <v>1</v>
+      </c>
+      <c r="K46" t="s">
+        <v>53</v>
+      </c>
+      <c r="L46" t="n">
+        <v>12816</v>
+      </c>
+      <c r="M46" t="n">
+        <v>0.1724</v>
+      </c>
+      <c r="N46" t="n">
+        <v>1</v>
+      </c>
+      <c r="O46" t="n">
+        <v>250.3291628551787</v>
+      </c>
+      <c r="P46" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
+      <c r="A47" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47" t="s">
+        <v>74</v>
+      </c>
+      <c r="C47" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" t="n">
+        <v>32</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" t="n">
+        <v>500</v>
+      </c>
+      <c r="G47" t="n">
+        <v>300</v>
+      </c>
+      <c r="H47" t="n">
+        <v>250</v>
+      </c>
+      <c r="I47" t="s">
+        <v>19</v>
+      </c>
+      <c r="J47" t="n">
+        <v>1</v>
+      </c>
+      <c r="K47" t="s">
+        <v>53</v>
+      </c>
+      <c r="L47" t="n">
+        <v>12816</v>
+      </c>
+      <c r="M47" t="n">
+        <v>0.1712</v>
+      </c>
+      <c r="N47" t="n">
+        <v>1</v>
+      </c>
+      <c r="O47" t="n">
+        <v>250.3291628551787</v>
+      </c>
+      <c r="P47" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
+      <c r="A48" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" t="s">
+        <v>75</v>
+      </c>
+      <c r="C48" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" t="n">
+        <v>32</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" t="n">
+        <v>500</v>
+      </c>
+      <c r="G48" t="n">
+        <v>300</v>
+      </c>
+      <c r="H48" t="n">
+        <v>250</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J48" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="K48" t="s">
+        <v>53</v>
+      </c>
+      <c r="L48" t="n">
+        <v>980</v>
+      </c>
+      <c r="M48" t="n">
+        <v>0.0301</v>
+      </c>
+      <c r="N48" t="n">
+        <v>0</v>
+      </c>
+      <c r="O48" t="s">
+        <v>19</v>
+      </c>
+      <c r="P48" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16">
+      <c r="A49" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" t="s">
+        <v>76</v>
+      </c>
+      <c r="C49" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49" t="n">
+        <v>32</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" t="n">
+        <v>500</v>
+      </c>
+      <c r="G49" t="n">
+        <v>300</v>
+      </c>
+      <c r="H49" t="n">
+        <v>250</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J49" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="K49" t="s">
+        <v>53</v>
+      </c>
+      <c r="L49" t="n">
+        <v>4046</v>
+      </c>
+      <c r="M49" t="n">
+        <v>0.06270000000000001</v>
+      </c>
+      <c r="N49" t="n">
+        <v>1</v>
+      </c>
+      <c r="O49" t="n">
+        <v>208.0402794253428</v>
+      </c>
+      <c r="P49" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16">
+      <c r="A50" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" t="s">
+        <v>77</v>
+      </c>
+      <c r="C50" t="s">
+        <v>18</v>
+      </c>
+      <c r="D50" t="n">
+        <v>32</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" t="n">
+        <v>500</v>
+      </c>
+      <c r="G50" t="n">
+        <v>300</v>
+      </c>
+      <c r="H50" t="n">
+        <v>250</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J50" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K50" t="s">
+        <v>53</v>
+      </c>
+      <c r="L50" t="n">
+        <v>2494</v>
+      </c>
+      <c r="M50" t="n">
+        <v>0.0532</v>
+      </c>
+      <c r="N50" t="n">
+        <v>1</v>
+      </c>
+      <c r="O50" t="n">
+        <v>35.80563434032669</v>
+      </c>
+      <c r="P50" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16">
+      <c r="A51" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" t="s">
+        <v>78</v>
+      </c>
+      <c r="C51" t="s">
+        <v>18</v>
+      </c>
+      <c r="D51" t="n">
+        <v>32</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" t="n">
+        <v>500</v>
+      </c>
+      <c r="G51" t="n">
+        <v>100</v>
+      </c>
+      <c r="H51" t="n">
+        <v>250</v>
+      </c>
+      <c r="I51" t="s">
+        <v>19</v>
+      </c>
+      <c r="J51" t="n">
+        <v>1</v>
+      </c>
+      <c r="K51" t="s">
+        <v>53</v>
+      </c>
+      <c r="L51" t="n">
+        <v>10335</v>
+      </c>
+      <c r="M51" t="n">
+        <v>0.2382</v>
+      </c>
+      <c r="N51" t="n">
+        <v>4</v>
+      </c>
+      <c r="O51" t="n">
+        <v>35.78592371085093</v>
+      </c>
+      <c r="P51" t="n">
+        <v>0.0144471012717442</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>79</v>
+      </c>
+      <c r="C52" t="s">
+        <v>18</v>
+      </c>
+      <c r="D52" t="n">
+        <v>32</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" t="n">
+        <v>500</v>
+      </c>
+      <c r="G52" t="n">
+        <v>100</v>
+      </c>
+      <c r="H52" t="n">
+        <v>250</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J52" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="K52" t="s">
+        <v>53</v>
+      </c>
+      <c r="L52" t="n">
+        <v>914</v>
+      </c>
+      <c r="M52" t="n">
+        <v>0.0321</v>
+      </c>
+      <c r="N52" t="n">
+        <v>0</v>
+      </c>
+      <c r="O52" t="s">
+        <v>19</v>
+      </c>
+      <c r="P52" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16">
+      <c r="A53" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>80</v>
+      </c>
+      <c r="C53" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" t="n">
+        <v>32</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0</v>
+      </c>
+      <c r="F53" t="n">
+        <v>500</v>
+      </c>
+      <c r="G53" t="n">
+        <v>100</v>
+      </c>
+      <c r="H53" t="n">
+        <v>250</v>
+      </c>
+      <c r="I53" t="s">
+        <v>19</v>
+      </c>
+      <c r="J53" t="n">
+        <v>1</v>
+      </c>
+      <c r="K53" t="s">
+        <v>53</v>
+      </c>
+      <c r="L53" t="n">
+        <v>10335</v>
+      </c>
+      <c r="M53" t="n">
+        <v>0.1495</v>
+      </c>
+      <c r="N53" t="n">
+        <v>4</v>
+      </c>
+      <c r="O53" t="n">
+        <v>35.78592371085093</v>
+      </c>
+      <c r="P53" t="n">
+        <v>0.0144471012717442</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16">
+      <c r="A54" t="s">
+        <v>51</v>
+      </c>
+      <c r="B54" t="s">
+        <v>81</v>
+      </c>
+      <c r="C54" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" t="n">
+        <v>32</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0</v>
+      </c>
+      <c r="F54" t="n">
+        <v>500</v>
+      </c>
+      <c r="G54" t="n">
+        <v>600</v>
+      </c>
+      <c r="H54" t="n">
+        <v>250</v>
+      </c>
+      <c r="I54" t="s">
+        <v>19</v>
+      </c>
+      <c r="J54" t="n">
+        <v>1</v>
+      </c>
+      <c r="K54" t="s">
+        <v>53</v>
+      </c>
+      <c r="L54" t="n">
+        <v>13704</v>
+      </c>
+      <c r="M54" t="n">
+        <v>0.1617</v>
+      </c>
+      <c r="N54" t="n">
+        <v>1</v>
+      </c>
+      <c r="O54" t="n">
+        <v>16.46900251232425</v>
+      </c>
+      <c r="P54" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16">
+      <c r="A55" t="s">
+        <v>51</v>
+      </c>
+      <c r="B55" t="s">
+        <v>82</v>
+      </c>
+      <c r="C55" t="s">
+        <v>18</v>
+      </c>
+      <c r="D55" t="n">
+        <v>32</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" t="n">
+        <v>500</v>
+      </c>
+      <c r="G55" t="n">
+        <v>50</v>
+      </c>
+      <c r="H55" t="n">
+        <v>250</v>
+      </c>
+      <c r="I55" t="s">
+        <v>19</v>
+      </c>
+      <c r="J55" t="n">
+        <v>1</v>
+      </c>
+      <c r="K55" t="s">
+        <v>53</v>
+      </c>
+      <c r="L55" t="n">
+        <v>6526</v>
+      </c>
+      <c r="M55" t="n">
+        <v>0.095</v>
+      </c>
+      <c r="N55" t="n">
+        <v>61</v>
+      </c>
+      <c r="O55" t="n">
+        <v>66.73192353300861</v>
+      </c>
+      <c r="P55" t="n">
+        <v>0.3268658760034935</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16">
+      <c r="A56" t="s">
+        <v>51</v>
+      </c>
+      <c r="B56" t="s">
+        <v>83</v>
+      </c>
+      <c r="C56" t="s">
+        <v>18</v>
+      </c>
+      <c r="D56" t="n">
+        <v>32</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" t="n">
+        <v>500</v>
+      </c>
+      <c r="G56" t="n">
+        <v>50</v>
+      </c>
+      <c r="H56" t="n">
+        <v>250</v>
+      </c>
+      <c r="I56" t="s">
+        <v>19</v>
+      </c>
+      <c r="J56" t="n">
+        <v>1</v>
+      </c>
+      <c r="K56" t="s">
+        <v>53</v>
+      </c>
+      <c r="L56" t="n">
+        <v>6526</v>
+      </c>
+      <c r="M56" t="n">
+        <v>0.0984</v>
+      </c>
+      <c r="N56" t="n">
+        <v>61</v>
+      </c>
+      <c r="O56" t="n">
+        <v>66.73192353300861</v>
+      </c>
+      <c r="P56" t="n">
+        <v>0.3268658760034935</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16">
+      <c r="A57" t="s">
+        <v>51</v>
+      </c>
+      <c r="B57" t="s">
+        <v>84</v>
+      </c>
+      <c r="C57" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" t="n">
+        <v>32</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" t="n">
+        <v>500</v>
+      </c>
+      <c r="G57" t="n">
+        <v>50</v>
+      </c>
+      <c r="H57" t="n">
+        <v>250</v>
+      </c>
+      <c r="I57" t="s">
+        <v>19</v>
+      </c>
+      <c r="J57" t="n">
+        <v>1</v>
+      </c>
+      <c r="K57" t="s">
+        <v>53</v>
+      </c>
+      <c r="L57" t="n">
+        <v>6526</v>
+      </c>
+      <c r="M57" t="n">
+        <v>0.093</v>
+      </c>
+      <c r="N57" t="n">
+        <v>61</v>
+      </c>
+      <c r="O57" t="n">
+        <v>66.73192353300861</v>
+      </c>
+      <c r="P57" t="n">
+        <v>0.3268658760034935</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16">
+      <c r="A58" t="s">
+        <v>51</v>
+      </c>
+      <c r="B58" t="s">
+        <v>85</v>
+      </c>
+      <c r="C58" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58" t="n">
+        <v>32</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G58" t="n">
+        <v>50</v>
+      </c>
+      <c r="H58" t="n">
+        <v>250</v>
+      </c>
+      <c r="I58" t="s">
+        <v>19</v>
+      </c>
+      <c r="J58" t="n">
+        <v>1</v>
+      </c>
+      <c r="K58" t="s">
+        <v>53</v>
+      </c>
+      <c r="L58" t="n">
+        <v>4684</v>
+      </c>
+      <c r="M58" t="n">
+        <v>0.0765</v>
+      </c>
+      <c r="N58" t="n">
+        <v>39</v>
+      </c>
+      <c r="O58" t="n">
+        <v>77.22859216835231</v>
+      </c>
+      <c r="P58" t="n">
+        <v>0.2213526034797603</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16">
+      <c r="A59" t="s">
+        <v>51</v>
+      </c>
+      <c r="B59" t="s">
+        <v>86</v>
+      </c>
+      <c r="C59" t="s">
+        <v>18</v>
+      </c>
+      <c r="D59" t="n">
+        <v>32</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0</v>
+      </c>
+      <c r="F59" t="n">
+        <v>500</v>
+      </c>
+      <c r="G59" t="n">
+        <v>100</v>
+      </c>
+      <c r="H59" t="n">
+        <v>250</v>
+      </c>
+      <c r="I59" t="s">
+        <v>19</v>
+      </c>
+      <c r="J59" t="n">
+        <v>1</v>
+      </c>
+      <c r="K59" t="s">
+        <v>53</v>
+      </c>
+      <c r="L59" t="n">
+        <v>10335</v>
+      </c>
+      <c r="M59" t="n">
+        <v>0.2086</v>
+      </c>
+      <c r="N59" t="n">
+        <v>4</v>
+      </c>
+      <c r="O59" t="n">
+        <v>35.78592371085093</v>
+      </c>
+      <c r="P59" t="n">
+        <v>0.0144471012717442</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16">
+      <c r="A60" t="s">
+        <v>51</v>
+      </c>
+      <c r="B60" t="s">
+        <v>87</v>
+      </c>
+      <c r="C60" t="s">
+        <v>18</v>
+      </c>
+      <c r="D60" t="n">
+        <v>32</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0</v>
+      </c>
+      <c r="F60" t="n">
+        <v>500</v>
+      </c>
+      <c r="G60" t="n">
+        <v>100</v>
+      </c>
+      <c r="H60" t="n">
+        <v>250</v>
+      </c>
+      <c r="I60" t="s">
+        <v>19</v>
+      </c>
+      <c r="J60" t="n">
+        <v>1</v>
+      </c>
+      <c r="K60" t="s">
+        <v>53</v>
+      </c>
+      <c r="L60" t="n">
+        <v>10335</v>
+      </c>
+      <c r="M60" t="n">
+        <v>0.1889</v>
+      </c>
+      <c r="N60" t="n">
+        <v>4</v>
+      </c>
+      <c r="O60" t="n">
+        <v>35.78592371085093</v>
+      </c>
+      <c r="P60" t="n">
+        <v>0.0144471012717442</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16">
+      <c r="A61" t="s">
+        <v>51</v>
+      </c>
+      <c r="B61" t="s">
+        <v>88</v>
+      </c>
+      <c r="C61" t="s">
+        <v>18</v>
+      </c>
+      <c r="D61" t="n">
+        <v>32</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0</v>
+      </c>
+      <c r="F61" t="n">
+        <v>500</v>
+      </c>
+      <c r="G61" t="n">
+        <v>100</v>
+      </c>
+      <c r="H61" t="n">
+        <v>250</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J61" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="K61" t="s">
+        <v>53</v>
+      </c>
+      <c r="L61" t="n">
+        <v>914</v>
+      </c>
+      <c r="M61" t="n">
+        <v>0.0331</v>
+      </c>
+      <c r="N61" t="n">
+        <v>0</v>
+      </c>
+      <c r="O61" t="s">
+        <v>19</v>
+      </c>
+      <c r="P61" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16">
+      <c r="A62" t="s">
+        <v>51</v>
+      </c>
+      <c r="B62" t="s">
+        <v>89</v>
+      </c>
+      <c r="C62" t="s">
+        <v>18</v>
+      </c>
+      <c r="D62" t="n">
+        <v>32</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0</v>
+      </c>
+      <c r="F62" t="n">
+        <v>500</v>
+      </c>
+      <c r="G62" t="n">
+        <v>100</v>
+      </c>
+      <c r="H62" t="n">
+        <v>250</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J62" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K62" t="s">
+        <v>53</v>
+      </c>
+      <c r="L62" t="n">
+        <v>1592</v>
+      </c>
+      <c r="M62" t="n">
+        <v>0.0376</v>
+      </c>
+      <c r="N62" t="n">
+        <v>1</v>
+      </c>
+      <c r="O62" t="n">
+        <v>127.517690301558</v>
+      </c>
+      <c r="P62" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16">
+      <c r="A63" t="s">
+        <v>51</v>
+      </c>
+      <c r="B63" t="s">
+        <v>90</v>
+      </c>
+      <c r="C63" t="s">
+        <v>18</v>
+      </c>
+      <c r="D63" t="n">
+        <v>32</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0</v>
+      </c>
+      <c r="F63" t="n">
+        <v>500</v>
+      </c>
+      <c r="G63" t="n">
+        <v>100</v>
+      </c>
+      <c r="H63" t="n">
+        <v>250</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J63" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="K63" t="s">
+        <v>53</v>
+      </c>
+      <c r="L63" t="n">
+        <v>914</v>
+      </c>
+      <c r="M63" t="n">
+        <v>0.0302</v>
+      </c>
+      <c r="N63" t="n">
+        <v>0</v>
+      </c>
+      <c r="O63" t="s">
+        <v>19</v>
+      </c>
+      <c r="P63" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16">
+      <c r="A64" t="s">
+        <v>51</v>
+      </c>
+      <c r="B64" t="s">
+        <v>91</v>
+      </c>
+      <c r="C64" t="s">
+        <v>18</v>
+      </c>
+      <c r="D64" t="n">
+        <v>32</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0</v>
+      </c>
+      <c r="F64" t="n">
+        <v>500</v>
+      </c>
+      <c r="G64" t="n">
+        <v>100</v>
+      </c>
+      <c r="H64" t="n">
+        <v>250</v>
+      </c>
+      <c r="I64" t="s">
+        <v>19</v>
+      </c>
+      <c r="J64" t="n">
+        <v>1</v>
+      </c>
+      <c r="K64" t="s">
+        <v>53</v>
+      </c>
+      <c r="L64" t="n">
+        <v>10335</v>
+      </c>
+      <c r="M64" t="n">
+        <v>0.1775</v>
+      </c>
+      <c r="N64" t="n">
+        <v>4</v>
+      </c>
+      <c r="O64" t="n">
+        <v>35.78592371085093</v>
+      </c>
+      <c r="P64" t="n">
+        <v>0.0144471012717442</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16">
+      <c r="A65" t="s">
+        <v>51</v>
+      </c>
+      <c r="B65" t="s">
+        <v>92</v>
+      </c>
+      <c r="C65" t="s">
+        <v>18</v>
+      </c>
+      <c r="D65" t="n">
+        <v>32</v>
+      </c>
+      <c r="E65" t="n">
+        <v>0</v>
+      </c>
+      <c r="F65" t="n">
+        <v>500</v>
+      </c>
+      <c r="G65" t="n">
+        <v>100</v>
+      </c>
+      <c r="H65" t="n">
+        <v>250</v>
+      </c>
+      <c r="I65" t="s">
+        <v>19</v>
+      </c>
+      <c r="J65" t="n">
+        <v>1</v>
+      </c>
+      <c r="K65" t="s">
+        <v>53</v>
+      </c>
+      <c r="L65" t="n">
+        <v>10335</v>
+      </c>
+      <c r="M65" t="n">
+        <v>0.1653</v>
+      </c>
+      <c r="N65" t="n">
+        <v>4</v>
+      </c>
+      <c r="O65" t="n">
+        <v>35.78592371085093</v>
+      </c>
+      <c r="P65" t="n">
+        <v>0.0144471012717442</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16">
+      <c r="A66" t="s">
+        <v>51</v>
+      </c>
+      <c r="B66" t="s">
+        <v>93</v>
+      </c>
+      <c r="C66" t="s">
+        <v>18</v>
+      </c>
+      <c r="D66" t="n">
+        <v>32</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0</v>
+      </c>
+      <c r="F66" t="n">
+        <v>500</v>
+      </c>
+      <c r="G66" t="n">
+        <v>100</v>
+      </c>
+      <c r="H66" t="n">
+        <v>250</v>
+      </c>
+      <c r="I66" t="s">
+        <v>19</v>
+      </c>
+      <c r="J66" t="n">
+        <v>1</v>
+      </c>
+      <c r="K66" t="s">
+        <v>53</v>
+      </c>
+      <c r="L66" t="n">
+        <v>10335</v>
+      </c>
+      <c r="M66" t="n">
+        <v>0.195</v>
+      </c>
+      <c r="N66" t="n">
+        <v>4</v>
+      </c>
+      <c r="O66" t="n">
+        <v>35.78592371085093</v>
+      </c>
+      <c r="P66" t="n">
+        <v>0.0144471012717442</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16">
+      <c r="A67" t="s">
+        <v>51</v>
+      </c>
+      <c r="B67" t="s">
+        <v>94</v>
+      </c>
+      <c r="C67" t="s">
+        <v>18</v>
+      </c>
+      <c r="D67" t="n">
+        <v>32</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0</v>
+      </c>
+      <c r="F67" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G67" t="n">
+        <v>100</v>
+      </c>
+      <c r="H67" t="n">
+        <v>250</v>
+      </c>
+      <c r="I67" t="s">
+        <v>19</v>
+      </c>
+      <c r="J67" t="n">
+        <v>1</v>
+      </c>
+      <c r="K67" t="s">
+        <v>53</v>
+      </c>
+      <c r="L67" t="n">
+        <v>9295</v>
+      </c>
+      <c r="M67" t="n">
+        <v>0.1318</v>
+      </c>
+      <c r="N67" t="n">
+        <v>5</v>
+      </c>
+      <c r="O67" t="n">
+        <v>39.84679002668249</v>
+      </c>
+      <c r="P67" t="n">
+        <v>0.02003501849434515</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16">
+      <c r="A68" t="s">
+        <v>51</v>
+      </c>
+      <c r="B68" t="s">
+        <v>95</v>
+      </c>
+      <c r="C68" t="s">
+        <v>18</v>
+      </c>
+      <c r="D68" t="n">
+        <v>32</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0</v>
+      </c>
+      <c r="F68" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G68" t="n">
+        <v>100</v>
+      </c>
+      <c r="H68" t="n">
+        <v>250</v>
+      </c>
+      <c r="I68" t="s">
+        <v>19</v>
+      </c>
+      <c r="J68" t="n">
+        <v>1</v>
+      </c>
+      <c r="K68" t="s">
+        <v>53</v>
+      </c>
+      <c r="L68" t="n">
+        <v>9295</v>
+      </c>
+      <c r="M68" t="n">
+        <v>0.1306</v>
+      </c>
+      <c r="N68" t="n">
+        <v>5</v>
+      </c>
+      <c r="O68" t="n">
+        <v>39.84679002668249</v>
+      </c>
+      <c r="P68" t="n">
+        <v>0.02003501849434515</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16">
+      <c r="A69" t="s">
+        <v>51</v>
+      </c>
+      <c r="B69" t="s">
+        <v>96</v>
+      </c>
+      <c r="C69" t="s">
+        <v>18</v>
+      </c>
+      <c r="D69" t="n">
+        <v>32</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0</v>
+      </c>
+      <c r="F69" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G69" t="n">
+        <v>100</v>
+      </c>
+      <c r="H69" t="n">
+        <v>250</v>
+      </c>
+      <c r="I69" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J69" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="K69" t="s">
+        <v>53</v>
+      </c>
+      <c r="L69" t="n">
+        <v>932</v>
+      </c>
+      <c r="M69" t="n">
+        <v>0.0412</v>
+      </c>
+      <c r="N69" t="n">
+        <v>0</v>
+      </c>
+      <c r="O69" t="s">
+        <v>19</v>
+      </c>
+      <c r="P69" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16">
+      <c r="A70" t="s">
+        <v>51</v>
+      </c>
+      <c r="B70" t="s">
+        <v>97</v>
+      </c>
+      <c r="C70" t="s">
+        <v>18</v>
+      </c>
+      <c r="D70" t="n">
+        <v>32</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F70" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G70" t="n">
+        <v>50</v>
+      </c>
+      <c r="H70" t="n">
+        <v>250</v>
+      </c>
+      <c r="I70" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J70" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="K70" t="s">
+        <v>53</v>
+      </c>
+      <c r="L70" t="n">
+        <v>563</v>
+      </c>
+      <c r="M70" t="n">
+        <v>0.0221</v>
+      </c>
+      <c r="N70" t="n">
+        <v>0</v>
+      </c>
+      <c r="O70" t="s">
+        <v>19</v>
+      </c>
+      <c r="P70" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16">
+      <c r="A71" t="s">
+        <v>51</v>
+      </c>
+      <c r="B71" t="s">
+        <v>98</v>
+      </c>
+      <c r="C71" t="s">
+        <v>18</v>
+      </c>
+      <c r="D71" t="n">
+        <v>32</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0</v>
+      </c>
+      <c r="F71" t="n">
+        <v>500</v>
+      </c>
+      <c r="G71" t="n">
+        <v>100</v>
+      </c>
+      <c r="H71" t="n">
+        <v>250</v>
+      </c>
+      <c r="I71" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J71" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="K71" t="s">
+        <v>53</v>
+      </c>
+      <c r="L71" t="n">
+        <v>10564</v>
+      </c>
+      <c r="M71" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="N71" t="n">
+        <v>3</v>
+      </c>
+      <c r="O71" t="n">
+        <v>40</v>
+      </c>
+      <c r="P71" t="n">
+        <v>0.01184249138684402</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>